<commit_message>
added models for 2017
</commit_message>
<xml_diff>
--- a/data/577 Projects/2012-2013/file list.xlsx
+++ b/data/577 Projects/2012-2013/file list.xlsx
@@ -492,14 +492,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="28.44140625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="28.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="42" style="4" customWidth="1"/>
-    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -550,7 +550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -567,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -584,7 +584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -601,7 +601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -618,7 +618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -635,7 +635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -652,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -669,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>

</xml_diff>